<commit_message>
add function to convert geo-time to Ma
</commit_message>
<xml_diff>
--- a/ChronostratChart2018-08.xlsx
+++ b/ChronostratChart2018-08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiasstal/proj/strat_chart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AFD20FE-524B-EB42-952B-4CDEF2957DBB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B458E7-5169-0B4C-B30E-D8FC6F71C2DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8280" yWindow="2860" windowWidth="27640" windowHeight="16940" xr2:uid="{5867EB8B-7289-B74C-B214-2B8D64A4B1C5}"/>
   </bookViews>
@@ -147,9 +147,6 @@
     <t>Uncertainty</t>
   </si>
   <si>
-    <t xml:space="preserve">age (Ma) </t>
-  </si>
-  <si>
     <t xml:space="preserve">Mesozoic </t>
   </si>
   <si>
@@ -559,6 +556,9 @@
   </si>
   <si>
     <t>Age</t>
+  </si>
+  <si>
+    <t>Ma</t>
   </si>
 </sst>
 </file>
@@ -931,11 +931,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5EA46F-9A2C-F446-B4F6-3A9A5902D3F7}">
-  <dimension ref="A1:J127"/>
+  <dimension ref="A1:J128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E103" sqref="E103"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -952,31 +952,31 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>175</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>38</v>
+        <v>175</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>37</v>
@@ -984,29 +984,17 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>168</v>
-      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
       <c r="H2" s="4">
-        <v>4.1999999999999997E-3</v>
+        <v>0</v>
       </c>
       <c r="I2" s="4"/>
-      <c r="J2" s="5"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="4"/>
@@ -1023,13 +1011,13 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H3" s="4">
-        <v>8.2000000000000007E-3</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="5"/>
@@ -1049,13 +1037,13 @@
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H4" s="4">
-        <v>1.17E-2</v>
+        <v>8.2000000000000007E-3</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="5"/>
@@ -1072,14 +1060,16 @@
         <v>7</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>167</v>
+      </c>
       <c r="H5" s="4">
-        <v>0.126</v>
+        <v>1.17E-2</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="5"/>
@@ -1099,11 +1089,11 @@
         <v>8</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="4">
-        <v>0.78100000000000003</v>
+        <v>0.126</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="5"/>
@@ -1122,14 +1112,12 @@
       <c r="E7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>168</v>
-      </c>
+      <c r="F7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="5"/>
       <c r="H7" s="4">
-        <v>1.8</v>
+        <v>0.78100000000000003</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="5"/>
@@ -1149,13 +1137,13 @@
         <v>8</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H8" s="4">
-        <v>2.58</v>
+        <v>1.8</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="5"/>
@@ -1169,19 +1157,19 @@
         <v>2</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H9" s="4">
-        <v>3.6</v>
+        <v>2.58</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
@@ -1201,13 +1189,13 @@
         <v>10</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H10" s="4">
-        <v>5.3330000000000002</v>
+        <v>3.6</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
@@ -1224,16 +1212,16 @@
         <v>9</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H11" s="4">
-        <v>7.2460000000000004</v>
+        <v>5.3330000000000002</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
@@ -1253,13 +1241,13 @@
         <v>11</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H12" s="4">
-        <v>11.63</v>
+        <v>7.2460000000000004</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
@@ -1278,14 +1266,14 @@
       <c r="E13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>19</v>
+      <c r="F13" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H13" s="4">
-        <v>13.82</v>
+        <v>11.63</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="5"/>
@@ -1305,11 +1293,13 @@
         <v>11</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>167</v>
+      </c>
       <c r="H14" s="4">
-        <v>15.97</v>
+        <v>13.82</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="5"/>
@@ -1328,12 +1318,12 @@
       <c r="E15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>21</v>
+      <c r="F15" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4">
-        <v>20.440000000000001</v>
+        <v>15.97</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="5"/>
@@ -1352,14 +1342,12 @@
       <c r="E16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>168</v>
-      </c>
+      <c r="F16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="4"/>
       <c r="H16" s="4">
-        <v>23.03</v>
+        <v>20.440000000000001</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="5"/>
@@ -1373,19 +1361,19 @@
         <v>2</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>28</v>
+        <v>11</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H17" s="4">
-        <v>27.82</v>
+        <v>23.03</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="5"/>
@@ -1405,13 +1393,13 @@
         <v>24</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H18" s="4">
-        <v>33.9</v>
+        <v>27.82</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="5"/>
@@ -1428,14 +1416,16 @@
         <v>27</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>167</v>
+      </c>
       <c r="H19" s="4">
-        <v>37.799999999999997</v>
+        <v>33.9</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="5"/>
@@ -1455,11 +1445,11 @@
         <v>25</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="G20" s="4"/>
       <c r="H20" s="4">
-        <v>41.2</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="5"/>
@@ -1479,13 +1469,11 @@
         <v>25</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>168</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="G21" s="5"/>
       <c r="H21" s="4">
-        <v>47.8</v>
+        <v>41.2</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="5"/>
@@ -1505,13 +1493,13 @@
         <v>25</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H22" s="4">
-        <v>56</v>
+        <v>47.8</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
@@ -1528,16 +1516,16 @@
         <v>27</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H23" s="4">
-        <v>59.2</v>
+        <v>56</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="5"/>
@@ -1557,13 +1545,13 @@
         <v>26</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H24" s="4">
-        <v>61.6</v>
+        <v>59.2</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="5"/>
@@ -1583,13 +1571,13 @@
         <v>26</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H25" s="4">
-        <v>66</v>
+        <v>61.6</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="5"/>
@@ -1600,27 +1588,25 @@
         <v>1</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H26" s="4">
-        <v>72.099999999999994</v>
+        <v>66</v>
       </c>
       <c r="I26" s="4"/>
-      <c r="J26" s="5">
-        <v>0.2</v>
-      </c>
+      <c r="J26" s="5"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="4"/>
@@ -1628,20 +1614,22 @@
         <v>1</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="F27" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G27" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>167</v>
+      </c>
       <c r="H27" s="4">
-        <v>83.6</v>
+        <v>72.099999999999994</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="5">
@@ -1654,26 +1642,24 @@
         <v>1</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="E28" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="F28" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>168</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="G28" s="5"/>
       <c r="H28" s="4">
-        <v>86.3</v>
+        <v>83.6</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="5">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1682,24 +1668,26 @@
         <v>1</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="F29" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G29" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>167</v>
+      </c>
       <c r="H29" s="4">
-        <v>89.8</v>
+        <v>86.3</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="5">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1708,25 +1696,25 @@
         <v>1</v>
       </c>
       <c r="C30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="F30" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>168</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="G30" s="5"/>
       <c r="H30" s="4">
-        <v>93.9</v>
+        <v>89.8</v>
       </c>
       <c r="I30" s="4"/>
-      <c r="J30" s="5"/>
+      <c r="J30" s="5">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="4"/>
@@ -1734,22 +1722,22 @@
         <v>1</v>
       </c>
       <c r="C31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="F31" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H31" s="4">
-        <v>100.5</v>
+        <v>93.9</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="5"/>
@@ -1760,26 +1748,24 @@
         <v>1</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="F32" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H32" s="4">
-        <v>113</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>169</v>
-      </c>
+        <v>100.5</v>
+      </c>
+      <c r="I32" s="4"/>
       <c r="J32" s="5"/>
     </row>
     <row r="33" spans="1:10">
@@ -1788,23 +1774,25 @@
         <v>1</v>
       </c>
       <c r="C33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="E33" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G33" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>167</v>
+      </c>
       <c r="H33" s="4">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J33" s="5"/>
     </row>
@@ -1814,23 +1802,23 @@
         <v>1</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="E34" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="4">
-        <v>129.4</v>
+        <v>125</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J34" s="5"/>
     </row>
@@ -1840,23 +1828,23 @@
         <v>1</v>
       </c>
       <c r="C35" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="E35" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G35" s="5"/>
       <c r="H35" s="4">
-        <v>132.9</v>
+        <v>129.4</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J35" s="5"/>
     </row>
@@ -1866,23 +1854,23 @@
         <v>1</v>
       </c>
       <c r="C36" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="E36" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G36" s="5"/>
       <c r="H36" s="4">
-        <v>139.80000000000001</v>
+        <v>132.9</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J36" s="5"/>
     </row>
@@ -1892,23 +1880,23 @@
         <v>1</v>
       </c>
       <c r="C37" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="E37" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G37" s="5"/>
       <c r="H37" s="4">
-        <v>145</v>
+        <v>139.80000000000001</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J37" s="5"/>
     </row>
@@ -1918,24 +1906,25 @@
         <v>1</v>
       </c>
       <c r="C38" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>13</v>
+      <c r="E38" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G38" s="5"/>
       <c r="H38" s="4">
-        <v>152.1</v>
-      </c>
-      <c r="J38" s="5">
-        <v>0.9</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="J38" s="5"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="4"/>
@@ -1943,23 +1932,23 @@
         <v>1</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G39" s="5"/>
-      <c r="H39" s="1">
-        <v>157.30000000000001</v>
+      <c r="H39" s="4">
+        <v>152.1</v>
       </c>
       <c r="J39" s="5">
-        <v>1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -1968,20 +1957,20 @@
         <v>1</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G40" s="5"/>
       <c r="H40" s="1">
-        <v>163.5</v>
+        <v>157.30000000000001</v>
       </c>
       <c r="J40" s="5">
         <v>1</v>
@@ -1993,23 +1982,23 @@
         <v>1</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G41" s="5"/>
       <c r="H41" s="1">
-        <v>166.1</v>
+        <v>163.5</v>
       </c>
       <c r="J41" s="5">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2018,25 +2007,23 @@
         <v>1</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>168</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G42" s="5"/>
       <c r="H42" s="1">
-        <v>168.3</v>
+        <v>166.1</v>
       </c>
       <c r="J42" s="5">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2045,25 +2032,25 @@
         <v>1</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H43" s="1">
-        <v>170.3</v>
+        <v>168.3</v>
       </c>
       <c r="J43" s="5">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2072,25 +2059,25 @@
         <v>1</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H44" s="1">
-        <v>174.1</v>
+        <v>170.3</v>
       </c>
       <c r="J44" s="5">
-        <v>1</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2099,25 +2086,25 @@
         <v>1</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H45" s="1">
-        <v>182.7</v>
+        <v>174.1</v>
       </c>
       <c r="J45" s="5">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2126,25 +2113,25 @@
         <v>1</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H46" s="1">
-        <v>190.8</v>
+        <v>182.7</v>
       </c>
       <c r="J46" s="5">
-        <v>1</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2153,25 +2140,25 @@
         <v>1</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H47" s="1">
-        <v>199.3</v>
+        <v>190.8</v>
       </c>
       <c r="J47" s="5">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2180,25 +2167,25 @@
         <v>1</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H48" s="1">
-        <v>201.3</v>
+        <v>199.3</v>
       </c>
       <c r="J48" s="5">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2207,25 +2194,26 @@
         <v>1</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G49" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>167</v>
+      </c>
       <c r="H49" s="1">
-        <v>208.5</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="J49" s="5"/>
+        <v>201.3</v>
+      </c>
+      <c r="J49" s="5">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="4"/>
@@ -2233,23 +2221,23 @@
         <v>1</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G50" s="5"/>
       <c r="H50" s="1">
-        <v>227</v>
+        <v>208.5</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J50" s="5"/>
     </row>
@@ -2259,25 +2247,23 @@
         <v>1</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G51" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G51" s="5"/>
+      <c r="H51" s="1">
+        <v>227</v>
+      </c>
+      <c r="I51" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="H51" s="1">
-        <v>237</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="J51" s="5"/>
     </row>
@@ -2287,25 +2273,25 @@
         <v>1</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G52" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="H52" s="1">
+        <v>237</v>
+      </c>
+      <c r="I52" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="H52" s="1">
-        <v>242</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="J52" s="5"/>
     </row>
@@ -2315,22 +2301,26 @@
         <v>1</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G53" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>167</v>
+      </c>
       <c r="H53" s="1">
-        <v>247.2</v>
-      </c>
-      <c r="I53" s="5"/>
+        <v>242</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>168</v>
+      </c>
       <c r="J53" s="5"/>
     </row>
     <row r="54" spans="1:10">
@@ -2339,20 +2329,20 @@
         <v>1</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G54" s="5"/>
       <c r="H54" s="1">
-        <v>251.2</v>
+        <v>247.2</v>
       </c>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
@@ -2363,54 +2353,50 @@
         <v>1</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="F55" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>168</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="G55" s="5"/>
       <c r="H55" s="1">
-        <v>251.90199999999999</v>
+        <v>251.2</v>
       </c>
       <c r="I55" s="5"/>
-      <c r="J55" s="1">
-        <v>2.4E-2</v>
-      </c>
+      <c r="J55" s="5"/>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="4"/>
       <c r="B56" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>77</v>
+      <c r="C56" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H56" s="1">
-        <v>254.14</v>
+        <v>251.90199999999999</v>
       </c>
       <c r="I56" s="5"/>
       <c r="J56" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>2.4E-2</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2419,26 +2405,26 @@
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="F57" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H57" s="1">
-        <v>259.10000000000002</v>
+        <v>254.14</v>
       </c>
       <c r="I57" s="5"/>
       <c r="J57" s="1">
-        <v>0.5</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2447,26 +2433,26 @@
         <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="E58" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="F58" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H58" s="1">
-        <v>265.10000000000002</v>
+        <v>259.10000000000002</v>
       </c>
       <c r="I58" s="5"/>
       <c r="J58" s="1">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2475,26 +2461,26 @@
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E59" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H59" s="1">
-        <v>268.8</v>
+        <v>265.10000000000002</v>
       </c>
       <c r="I59" s="5"/>
       <c r="J59" s="1">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -2503,26 +2489,26 @@
         <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E60" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H60" s="1">
-        <v>272.95</v>
+        <v>268.8</v>
       </c>
       <c r="I60" s="5"/>
       <c r="J60" s="1">
-        <v>0.11</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -2531,24 +2517,26 @@
         <v>1</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E61" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G61" s="5"/>
+        <v>85</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>167</v>
+      </c>
       <c r="H61" s="1">
-        <v>283.5</v>
+        <v>272.95</v>
       </c>
       <c r="I61" s="5"/>
       <c r="J61" s="1">
-        <v>0.6</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2557,24 +2545,24 @@
         <v>1</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E62" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G62" s="5"/>
       <c r="H62" s="1">
-        <v>290.10000000000002</v>
+        <v>283.5</v>
       </c>
       <c r="I62" s="5"/>
       <c r="J62" s="1">
-        <v>0.26</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2583,26 +2571,24 @@
         <v>1</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E63" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G63" s="5" t="s">
-        <v>168</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G63" s="5"/>
       <c r="H63" s="1">
-        <v>293.52</v>
+        <v>290.10000000000002</v>
       </c>
       <c r="I63" s="5"/>
       <c r="J63" s="1">
-        <v>0.17</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -2611,26 +2597,26 @@
         <v>1</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E64" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H64" s="1">
-        <v>298.89999999999998</v>
+        <v>293.52</v>
       </c>
       <c r="I64" s="5"/>
       <c r="J64" s="1">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -2639,24 +2625,26 @@
         <v>1</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="E65" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G65" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>167</v>
+      </c>
       <c r="H65" s="1">
-        <v>303.7</v>
+        <v>298.89999999999998</v>
       </c>
       <c r="I65" s="5"/>
-      <c r="J65" s="4">
-        <v>0.1</v>
+      <c r="J65" s="1">
+        <v>0.15</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -2665,20 +2653,20 @@
         <v>1</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D66" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E66" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="F66" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G66" s="5"/>
       <c r="H66" s="1">
-        <v>307</v>
+        <v>303.7</v>
       </c>
       <c r="I66" s="5"/>
       <c r="J66" s="4">
@@ -2691,24 +2679,24 @@
         <v>1</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D67" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="F67" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G67" s="5"/>
       <c r="H67" s="1">
-        <v>315.2</v>
+        <v>307</v>
       </c>
       <c r="I67" s="5"/>
       <c r="J67" s="4">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -2717,26 +2705,24 @@
         <v>1</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>168</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="G68" s="5"/>
       <c r="H68" s="1">
-        <v>323.2</v>
+        <v>315.2</v>
       </c>
       <c r="I68" s="5"/>
       <c r="J68" s="4">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -2745,24 +2731,26 @@
         <v>1</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G69" s="5"/>
+        <v>100</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>167</v>
+      </c>
       <c r="H69" s="1">
-        <v>330.9</v>
+        <v>323.2</v>
       </c>
       <c r="I69" s="5"/>
       <c r="J69" s="4">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -2771,26 +2759,24 @@
         <v>1</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="H70" s="4">
-        <v>346.7</v>
+        <v>101</v>
+      </c>
+      <c r="G70" s="5"/>
+      <c r="H70" s="1">
+        <v>330.9</v>
       </c>
       <c r="I70" s="5"/>
       <c r="J70" s="4">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -2799,22 +2785,22 @@
         <v>1</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H71" s="4">
-        <v>358.9</v>
+        <v>346.7</v>
       </c>
       <c r="I71" s="5"/>
       <c r="J71" s="4">
@@ -2827,26 +2813,26 @@
         <v>1</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="H72" s="1">
-        <v>372.2</v>
+        <v>167</v>
+      </c>
+      <c r="H72" s="4">
+        <v>358.9</v>
       </c>
       <c r="I72" s="5"/>
       <c r="J72" s="4">
-        <v>1.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -2855,22 +2841,22 @@
         <v>1</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D73" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E73" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="G73" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H73" s="1">
-        <v>382.7</v>
+        <v>372.2</v>
       </c>
       <c r="I73" s="5"/>
       <c r="J73" s="4">
@@ -2883,26 +2869,26 @@
         <v>1</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>14</v>
+        <v>104</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H74" s="1">
-        <v>387.7</v>
+        <v>382.7</v>
       </c>
       <c r="I74" s="5"/>
       <c r="J74" s="4">
-        <v>0.8</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -2911,26 +2897,26 @@
         <v>1</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H75" s="1">
-        <v>393.3</v>
+        <v>387.7</v>
       </c>
       <c r="I75" s="5"/>
       <c r="J75" s="4">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -2939,26 +2925,26 @@
         <v>1</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H76" s="1">
-        <v>407.6</v>
+        <v>393.3</v>
       </c>
       <c r="I76" s="5"/>
       <c r="J76" s="4">
-        <v>2.6</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -2967,26 +2953,26 @@
         <v>1</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H77" s="1">
-        <v>410.8</v>
+        <v>407.6</v>
       </c>
       <c r="I77" s="5"/>
       <c r="J77" s="4">
-        <v>2.8</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -2995,26 +2981,26 @@
         <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H78" s="1">
-        <v>419.2</v>
+        <v>410.8</v>
       </c>
       <c r="I78" s="5"/>
       <c r="J78" s="4">
-        <v>3.2</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -3023,24 +3009,26 @@
         <v>1</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F79" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="G79" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H79" s="1">
-        <v>423</v>
+        <v>419.2</v>
       </c>
       <c r="I79" s="5"/>
       <c r="J79" s="4">
-        <v>2.2999999999999998</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -3049,26 +3037,24 @@
         <v>1</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D80" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E80" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>119</v>
-      </c>
+      <c r="F80" s="5"/>
       <c r="G80" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H80" s="1">
-        <v>425.6</v>
+        <v>423</v>
       </c>
       <c r="I80" s="5"/>
       <c r="J80" s="4">
-        <v>0.9</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -3077,26 +3063,26 @@
         <v>1</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H81" s="1">
-        <v>427.4</v>
+        <v>425.6</v>
       </c>
       <c r="I81" s="5"/>
       <c r="J81" s="4">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -3105,26 +3091,26 @@
         <v>1</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H82" s="1">
-        <v>430.5</v>
+        <v>427.4</v>
       </c>
       <c r="I82" s="5"/>
       <c r="J82" s="4">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -3133,26 +3119,26 @@
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H83" s="1">
-        <v>433.4</v>
+        <v>430.5</v>
       </c>
       <c r="I83" s="5"/>
       <c r="J83" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -3161,26 +3147,26 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H84" s="1">
-        <v>438.5</v>
+        <v>433.4</v>
       </c>
       <c r="I84" s="5"/>
       <c r="J84" s="4">
-        <v>1.1000000000000001</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -3189,26 +3175,26 @@
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H85" s="1">
-        <v>440.8</v>
+        <v>438.5</v>
       </c>
       <c r="I85" s="5"/>
       <c r="J85" s="4">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -3217,26 +3203,26 @@
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H86" s="1">
-        <v>443.8</v>
+        <v>440.8</v>
       </c>
       <c r="I86" s="5"/>
       <c r="J86" s="4">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -3245,26 +3231,26 @@
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>41</v>
+        <v>111</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H87" s="1">
-        <v>445.2</v>
+        <v>443.8</v>
       </c>
       <c r="I87" s="5"/>
       <c r="J87" s="4">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -3273,26 +3259,26 @@
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D88" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E88" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="G88" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H88" s="1">
-        <v>453</v>
+        <v>445.2</v>
       </c>
       <c r="I88" s="5"/>
       <c r="J88" s="4">
-        <v>0.7</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -3301,26 +3287,26 @@
         <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H89" s="1">
-        <v>458.4</v>
+        <v>453</v>
       </c>
       <c r="I89" s="5"/>
       <c r="J89" s="4">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -3329,26 +3315,26 @@
         <v>1</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>14</v>
+        <v>125</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H90" s="1">
-        <v>467.3</v>
+        <v>458.4</v>
       </c>
       <c r="I90" s="5"/>
       <c r="J90" s="4">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -3357,26 +3343,26 @@
         <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E91" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H91" s="1">
-        <v>470</v>
+        <v>467.3</v>
       </c>
       <c r="I91" s="5"/>
       <c r="J91" s="4">
-        <v>1.4</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -3385,22 +3371,22 @@
         <v>1</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H92" s="1">
-        <v>477.7</v>
+        <v>470</v>
       </c>
       <c r="I92" s="5"/>
       <c r="J92" s="4">
@@ -3413,26 +3399,26 @@
         <v>1</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H93" s="1">
-        <v>485.4</v>
+        <v>477.7</v>
       </c>
       <c r="I93" s="5"/>
       <c r="J93" s="4">
-        <v>1.9</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -3441,25 +3427,27 @@
         <v>1</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G94" s="5"/>
+        <v>125</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>167</v>
+      </c>
       <c r="H94" s="1">
-        <v>489.5</v>
-      </c>
-      <c r="I94" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="J94" s="5"/>
+        <v>485.4</v>
+      </c>
+      <c r="I94" s="5"/>
+      <c r="J94" s="4">
+        <v>1.9</v>
+      </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="4"/>
@@ -3467,25 +3455,23 @@
         <v>1</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D95" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E95" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E95" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G95" s="5" t="s">
+      <c r="F95" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G95" s="5"/>
+      <c r="H95" s="1">
+        <v>489.5</v>
+      </c>
+      <c r="I95" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="H95" s="1">
-        <v>494</v>
-      </c>
-      <c r="I95" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="J95" s="5"/>
     </row>
@@ -3495,25 +3481,25 @@
         <v>1</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D96" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E96" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E96" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="F96" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G96" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="H96" s="1">
+        <v>494</v>
+      </c>
+      <c r="I96" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="H96" s="1">
-        <v>497</v>
-      </c>
-      <c r="I96" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="J96" s="5"/>
     </row>
@@ -3523,25 +3509,25 @@
         <v>1</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D97" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E97" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E97" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="F97" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G97" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="H97" s="1">
+        <v>497</v>
+      </c>
+      <c r="I97" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="H97" s="1">
-        <v>500.5</v>
-      </c>
-      <c r="I97" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="J97" s="5"/>
     </row>
@@ -3551,25 +3537,25 @@
         <v>1</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G98" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="H98" s="1">
+        <v>500.5</v>
+      </c>
+      <c r="I98" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="H98" s="1">
-        <v>504.5</v>
-      </c>
-      <c r="I98" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="J98" s="5"/>
     </row>
@@ -3579,26 +3565,27 @@
         <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G99" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="H99" s="1">
+        <v>504.5</v>
+      </c>
+      <c r="I99" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="H99" s="1">
-        <v>509</v>
-      </c>
-      <c r="I99" s="5" t="s">
-        <v>169</v>
-      </c>
+      <c r="J99" s="5"/>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="4"/>
@@ -3606,22 +3593,25 @@
         <v>1</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>143</v>
+        <v>133</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>167</v>
       </c>
       <c r="H100" s="1">
-        <v>514</v>
-      </c>
-      <c r="I100" s="2" t="s">
-        <v>169</v>
+        <v>509</v>
+      </c>
+      <c r="I100" s="5" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -3630,22 +3620,22 @@
         <v>1</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H101" s="1">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="102" spans="1:10">
@@ -3654,22 +3644,22 @@
         <v>1</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>118</v>
+        <v>133</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H102" s="1">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="103" spans="1:10">
@@ -3678,281 +3668,300 @@
         <v>1</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G103" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="H103" s="1">
+        <v>529</v>
+      </c>
+      <c r="I103" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H103" s="1">
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104" s="4"/>
+      <c r="B104" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H104" s="1">
         <v>541</v>
       </c>
-      <c r="J103" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10">
-      <c r="A104" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H104" s="1">
-        <v>635</v>
-      </c>
-      <c r="I104" s="2" t="s">
-        <v>169</v>
+      <c r="J104" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="C105" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="D105" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="H105" s="1">
-        <v>720</v>
+        <v>635</v>
       </c>
       <c r="I105" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="C106" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="D106" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H106" s="1">
-        <v>1000</v>
+        <v>720</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="C107" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="D107" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H107" s="1">
-        <v>1200</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="108" spans="1:10">
       <c r="A108" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="C108" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H108" s="1">
-        <v>1400</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="C109" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H109" s="1">
-        <v>1600</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="110" spans="1:10">
       <c r="A110" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="C110" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H110" s="1">
-        <v>1800</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="111" spans="1:10">
       <c r="A111" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="C111" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H111" s="1">
-        <v>2050</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="112" spans="1:10">
       <c r="A112" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="C112" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H112" s="1">
-        <v>2300</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="113" spans="1:8">
       <c r="A113" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B113" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B113" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="C113" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H113" s="1">
-        <v>2500</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="114" spans="1:8">
       <c r="A114" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B114" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="C114" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="H114" s="2">
-        <v>2800</v>
+        <v>150</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H114" s="1">
+        <v>2500</v>
       </c>
     </row>
     <row r="115" spans="1:8">
       <c r="A115" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H115" s="2">
-        <v>3200</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="116" spans="1:8">
       <c r="A116" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H116" s="2">
-        <v>3600</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="117" spans="1:8">
       <c r="A117" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H117" s="2">
-        <v>4000</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="118" spans="1:8">
       <c r="A118" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
-      <c r="E118" s="1"/>
-      <c r="F118" s="1"/>
+        <v>151</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="H118" s="2">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+      <c r="F119" s="1"/>
+      <c r="H119" s="2">
         <v>4600</v>
       </c>
-    </row>
-    <row r="119" spans="1:8">
-      <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
-      <c r="C119" s="1"/>
     </row>
     <row r="120" spans="1:8">
       <c r="A120" s="1"/>
@@ -3976,6 +3985,8 @@
     </row>
     <row r="124" spans="1:8">
       <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="1"/>
     </row>
     <row r="125" spans="1:8">
       <c r="A125" s="1"/>
@@ -3985,6 +3996,9 @@
     </row>
     <row r="127" spans="1:8">
       <c r="A127" s="1"/>
+    </row>
+    <row r="128" spans="1:8">
+      <c r="A128" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>